<commit_message>
Top k Frequent elements-buckets
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA8A9B-4F16-49A4-8455-DC6E8D1366F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E67272-208E-4E06-A18E-A83B3640A432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{379DC1C9-35C1-443A-8BE3-39CE01DBA4F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Category</t>
   </si>
@@ -90,6 +90,19 @@
   </si>
   <si>
     <t>O(n) for creation of the counter. Note list creation at the end of the k elements takes O(k) spacd but typically n is much greater than k thus O(n) dominates</t>
+  </si>
+  <si>
+    <t>Use a min_heap to store the freq, num in the min_heap and keep it of size k. Finally return the min_heap</t>
+  </si>
+  <si>
+    <t>For each of the distinct elements (at most n), we perform heap operations that take O(log k) time. So overll time complexity in O(n* log k)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The space complexity is O(n):
+The Counter object requires O(n) space in the worst case (when all elements are unique).
+The heap requires O(k) space.
+Since n ≥ k, the overall space complexity is dominated by O(n).
+</t>
   </si>
 </sst>
 </file>
@@ -142,7 +155,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,44 +496,45 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.90625" customWidth="1"/>
-    <col min="4" max="4" width="74" customWidth="1"/>
-    <col min="5" max="5" width="32.90625" customWidth="1"/>
-    <col min="6" max="6" width="51.90625" customWidth="1"/>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="51.90625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -534,34 +550,43 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>347</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>347</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -572,5 +597,6 @@
     <hyperlink ref="C2" r:id="rId3" display="https://leetcode.com/problems/group-anagrams/" xr:uid="{C0450B54-F946-4A43-8AE8-FE782D8AB0D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Encode and decode strings
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E67272-208E-4E06-A18E-A83B3640A432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1301C57-94BD-444C-9AC4-A6F615C69F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{379DC1C9-35C1-443A-8BE3-39CE01DBA4F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Category</t>
   </si>
@@ -103,6 +103,22 @@
 The heap requires O(k) space.
 Since n ≥ k, the overall space complexity is dominated by O(n).
 </t>
+  </si>
+  <si>
+    <t>Encode and Decode Strings</t>
+  </si>
+  <si>
+    <t>Encoding: Calculate a 4 string format for length of string. Append Length+string for each of the string oin list
+Decoding : First slice the 4 string to extract length of the string and then select the string. Move on to the next Length+string combo and repeat</t>
+  </si>
+  <si>
+    <t>Space Complexity: O(L + n) for encoding and O(L) for decoding</t>
+  </si>
+  <si>
+    <t>Time Complexity: O(n + L) for encoding and O(L) for decoding
+where
+n is the number of strings
+L is the total length of all strings combined</t>
   </si>
 </sst>
 </file>
@@ -147,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -157,6 +173,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -493,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAD0A2B-7174-4393-8E63-B77E3A1E3BD1}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,13 +609,34 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>271</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="https://leetcode.com/problems/top-k-frequent-elements/" xr:uid="{681E1671-DC0B-47D9-A85E-3F1F5E1FBEAE}"/>
     <hyperlink ref="C4" r:id="rId2" display="https://leetcode.com/problems/top-k-frequent-elements/" xr:uid="{274D70F2-43D2-4226-BC83-BAD5CEA957D1}"/>
     <hyperlink ref="C2" r:id="rId3" display="https://leetcode.com/problems/group-anagrams/" xr:uid="{C0450B54-F946-4A43-8AE8-FE782D8AB0D0}"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://leetcode.com/problems/encode-and-decode-strings" xr:uid="{A063A06F-9EBB-4AA9-B80C-A543256BF4E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
longest non repeating subsequence
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E8D9C1-3BCB-46E8-A522-95406064F984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B2A9D6-8E83-41F6-A9CF-2213CF68DD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{379DC1C9-35C1-443A-8BE3-39CE01DBA4F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Category</t>
   </si>
@@ -131,6 +131,22 @@
   </si>
   <si>
     <t>O(1) since we only use constant amount of space</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays </t>
+  </si>
+  <si>
+    <t>Brute Force - Check all the substring one by one to see if it has no duplicate character.</t>
+  </si>
+  <si>
+    <t>Brute Force - O(n**3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brute Force - The space taken by the char set O(min(n,m) where n in the length of the string and m is the char set (128 for ASCII , 26 for smaller alphabets
+</t>
   </si>
 </sst>
 </file>
@@ -525,17 +541,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAD0A2B-7174-4393-8E63-B77E3A1E3BD1}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="74" style="1" customWidth="1"/>
     <col min="5" max="5" width="32.90625" style="1" customWidth="1"/>
     <col min="6" max="6" width="51.90625" style="1" customWidth="1"/>
@@ -643,6 +659,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B6" s="1">
         <v>238</v>
       </c>
@@ -657,6 +676,26 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -666,8 +705,9 @@
     <hyperlink ref="C2" r:id="rId3" display="https://leetcode.com/problems/group-anagrams/" xr:uid="{C0450B54-F946-4A43-8AE8-FE782D8AB0D0}"/>
     <hyperlink ref="C5" r:id="rId4" display="https://leetcode.com/problems/encode-and-decode-strings" xr:uid="{A063A06F-9EBB-4AA9-B80C-A543256BF4E4}"/>
     <hyperlink ref="C6" r:id="rId5" display="https://leetcode.com/problems/product-of-array-except-self/" xr:uid="{CF343F4E-FEF0-40E0-9959-0A92CA385D07}"/>
+    <hyperlink ref="C7" r:id="rId6" display="https://leetcode.com/problems/longest-substring-without-repeating-characters/" xr:uid="{F03BA630-2C59-4CCB-A744-F46C15050644}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Max path binary sum
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96818C38-5992-4906-B3A7-37AFC6C92982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD24BB6C-B7D1-4EFF-82D5-FB6F8B6B23A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{379DC1C9-35C1-443A-8BE3-39CE01DBA4F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Category</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>#Post traversal
+Do a dfs
+Keep max_sum which should be the sum of the left max path and the right max path + the node val
+#remember when you return you will return only the node.val and max of left_sum or right_sum. reason is as you pass on the value to the root you can only pass left or right max path</t>
+  </si>
+  <si>
+    <t>dfs visits each node and hence time complexity is O(n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The main factor contributing to the space complexity (beyond the storage for the tree itself) is the recursion call stack used by the dfs function. The maximum depth of the recursion call stack corresponds to the height (H) of the binary tree. . Worst case it is a skewed </t>
   </si>
 </sst>
 </file>
@@ -546,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAD0A2B-7174-4393-8E63-B77E3A1E3BD1}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -701,12 +713,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>124</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
graph to linked list
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD24BB6C-B7D1-4EFF-82D5-FB6F8B6B23A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FED179-0323-4705-8E54-F8885582C6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{379DC1C9-35C1-443A-8BE3-39CE01DBA4F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Category</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t xml:space="preserve"> The main factor contributing to the space complexity (beyond the storage for the tree itself) is the recursion call stack used by the dfs function. The maximum depth of the recursion call stack corresponds to the height (H) of the binary tree. . Worst case it is a skewed </t>
+  </si>
+  <si>
+    <t>Tree and Graphs</t>
+  </si>
+  <si>
+    <t>Binary Tree Right Side View</t>
   </si>
 </sst>
 </file>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAD0A2B-7174-4393-8E63-B77E3A1E3BD1}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -730,6 +736,17 @@
         <v>35</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1">
+        <v>199</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="https://leetcode.com/problems/top-k-frequent-elements/" xr:uid="{681E1671-DC0B-47D9-A85E-3F1F5E1FBEAE}"/>
@@ -739,8 +756,9 @@
     <hyperlink ref="C6" r:id="rId5" display="https://leetcode.com/problems/product-of-array-except-self/" xr:uid="{CF343F4E-FEF0-40E0-9959-0A92CA385D07}"/>
     <hyperlink ref="C7" r:id="rId6" display="https://leetcode.com/problems/longest-substring-without-repeating-characters/" xr:uid="{F03BA630-2C59-4CCB-A744-F46C15050644}"/>
     <hyperlink ref="C8" r:id="rId7" display="https://leetcode.com/problems/binary-tree-maximum-path-sum/" xr:uid="{1AC349A6-E494-4B7B-8227-2E33E2081569}"/>
+    <hyperlink ref="C9" r:id="rId8" display="https://leetcode.com/problems/binary-tree-right-side-view/" xr:uid="{4208EADF-904A-4295-85BA-F8088FEFD256}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lowes common ancestor 111
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC1EC09-B71B-4F13-ADD9-B0CC09F05589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8549EF5-2217-43D4-B611-E8B2D75924A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{379DC1C9-35C1-443A-8BE3-39CE01DBA4F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Category</t>
   </si>
@@ -223,6 +223,33 @@
   </si>
   <si>
     <t>min heap solution presented in the original code is O(n), where n is the number of elements in the input array nums.</t>
+  </si>
+  <si>
+    <t>Basic Calculator II</t>
+  </si>
+  <si>
+    <t>use a stack and value and last operator. Then enumerate through the string, update value if char is digit, if char is not a number, check the last operator and append value to the stack accordingly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O(n) as we iterate through each character of the input string exactly once
+</t>
+  </si>
+  <si>
+    <t>The space complexity is determined by the stack storage:
+In the worst case, every other character could be a number followed by a '+' or '-' operator, resulting in a stack with approximately n/2 elements. Hence space complexity in O(n)</t>
+  </si>
+  <si>
+    <t> Lowest Common Ancestor of a Binary Tree III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use two pointers a,b mapped to p,q and traverse to their respective parents.one its reaches parents point them to q, p. Return a </t>
+  </si>
+  <si>
+    <t>Each pointer might traverse at most 2h nodes, where h is the height of the tree. Since we're considering the asymptotic complexity, this simplifies to O(h). For a balanced binary tree, h would be log(n) where n is the number of nodes, making the time complexity O(log n). However, in the worst case of a skewed tree, h could be n, making the time complexity O(n)</t>
+  </si>
+  <si>
+    <t>The space complexity is O(1) or constant space because:
+The algorithm only uses two pointers ('a' and 'b') regardless of the input size.</t>
   </si>
 </sst>
 </file>
@@ -617,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAD0A2B-7174-4393-8E63-B77E3A1E3BD1}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -871,6 +898,46 @@
         <v>55</v>
       </c>
     </row>
+    <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1">
+        <v>227</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1650</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="https://leetcode.com/problems/top-k-frequent-elements/" xr:uid="{681E1671-DC0B-47D9-A85E-3F1F5E1FBEAE}"/>
@@ -884,8 +951,10 @@
     <hyperlink ref="C10" r:id="rId9" display="https://leetcode.com/problems/minimum-remove-to-make-valid-parentheses/" xr:uid="{B1BFC614-2576-41CA-B4AA-E2D137ED8FD2}"/>
     <hyperlink ref="C11" r:id="rId10" display="https://leetcode.com/problems/valid-palindrome-ii/" xr:uid="{AEDDCEEF-3247-4F37-BC0D-578A3A5B434C}"/>
     <hyperlink ref="C12" r:id="rId11" display="https://leetcode.com/problems/kth-largest-element-in-an-array/" xr:uid="{75F78499-BA0C-44E2-9FB3-329723B2412B}"/>
+    <hyperlink ref="C13" r:id="rId12" display="https://leetcode.com/problems/basic-calculator-ii/" xr:uid="{8DBA1D9F-FCC4-417A-9403-DC18CA8527B7}"/>
+    <hyperlink ref="C14" r:id="rId13" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree-iii/" xr:uid="{EA7FDFE9-EC2C-4ED0-882A-A6F9A5E3D200}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Random pick with weight
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8549EF5-2217-43D4-B611-E8B2D75924A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90333D36-10F7-414C-B8C1-90C60AEB381B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{379DC1C9-35C1-443A-8BE3-39CE01DBA4F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t>Category</t>
   </si>
@@ -250,6 +250,26 @@
   <si>
     <t>The space complexity is O(1) or constant space because:
 The algorithm only uses two pointers ('a' and 'b') regardless of the input size.</t>
+  </si>
+  <si>
+    <t>Nested List Weight Sum</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t> We go through the list of nested integers one by one, keeping track of the current depth d. If a nested integer is an integer, n, we calculate its sum as n×d. If the nested integer is a list, we calculate the sum of this list recursively using the same process but with depth equals d+1.</t>
+  </si>
+  <si>
+    <t>Recursion stack - O(n)</t>
+  </si>
+  <si>
+    <t>The space complexity of this solution is O(d), where d is the maximum depth of the nested list.
+This is due to:
+The recursive nature of the DFS implementation
+Each recursive call adds a new frame to the call stack
+The maximum number of frames on the call stack at any given time corresponds to the maximum depth of the nested list
+No additional data structures are used that grow with the input size</t>
   </si>
 </sst>
 </file>
@@ -644,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAD0A2B-7174-4393-8E63-B77E3A1E3BD1}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,6 +958,26 @@
         <v>63</v>
       </c>
     </row>
+    <row r="15" spans="1:6" ht="203" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1">
+        <v>339</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="https://leetcode.com/problems/top-k-frequent-elements/" xr:uid="{681E1671-DC0B-47D9-A85E-3F1F5E1FBEAE}"/>
@@ -953,8 +993,9 @@
     <hyperlink ref="C12" r:id="rId11" display="https://leetcode.com/problems/kth-largest-element-in-an-array/" xr:uid="{75F78499-BA0C-44E2-9FB3-329723B2412B}"/>
     <hyperlink ref="C13" r:id="rId12" display="https://leetcode.com/problems/basic-calculator-ii/" xr:uid="{8DBA1D9F-FCC4-417A-9403-DC18CA8527B7}"/>
     <hyperlink ref="C14" r:id="rId13" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree-iii/" xr:uid="{EA7FDFE9-EC2C-4ED0-882A-A6F9A5E3D200}"/>
+    <hyperlink ref="C15" r:id="rId14" display="https://leetcode.com/problems/nested-list-weight-sum/" xr:uid="{1A063C60-CD9B-41E0-BCB7-34048AD51C7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>